<commit_message>
Fixed LZ77 last byte bug
</commit_message>
<xml_diff>
--- a/DATA/results (version 1).xlsx
+++ b/DATA/results (version 1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\newap\CLionProjects\HW_Archiver\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA302A0-B3AD-4F40-A206-B38035CE01A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5D8156-D52F-415E-BF78-4E5A4EF4672F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="1932" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Частоты появления символов в фа" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="17">
   <si>
     <t>Файл</t>
   </si>
@@ -142,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -156,6 +158,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2582,7 +2589,7 @@
                   <c:v>0.50864262171506058</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.224563106938371E-2</c:v>
+                  <c:v>6.2246119477266812E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.4461946053326002</c:v>
@@ -2640,7 +2647,7 @@
                   <c:v>1.8107131502271285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.49676375247344895</c:v>
+                  <c:v>0.49676423817771531</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6.2546001917489352E-2</c:v>
@@ -21361,33 +21368,33 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
       <c r="O2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -41447,10 +41454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57817B2E-75C9-4DF5-99DC-7BEE068933E1}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="68" workbookViewId="0">
-      <selection sqref="A1:M14"/>
+    <sheetView tabSelected="1" topLeftCell="G3" zoomScale="68" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41459,73 +41466,140 @@
     <col min="7" max="7" width="15.5546875" customWidth="1"/>
     <col min="9" max="9" width="17.44140625" customWidth="1"/>
     <col min="11" max="11" width="17.109375" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" customWidth="1"/>
+    <col min="16" max="16" width="5.44140625" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" s="12"/>
+      <c r="U1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB1" s="11"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
         <v>12</v>
       </c>
@@ -41556,8 +41630,41 @@
       <c r="M4" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -41602,8 +41709,52 @@
         <f>$L5/$B5</f>
         <v>1.4387643855659011</v>
       </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>2107842</v>
+      </c>
+      <c r="R5" s="3">
+        <v>-41251.9</v>
+      </c>
+      <c r="S5" s="9">
+        <v>2110330</v>
+      </c>
+      <c r="T5" s="8">
+        <f>$D5/$B5</f>
+        <v>1.0011803541252142</v>
+      </c>
+      <c r="U5" s="9">
+        <v>3942894</v>
+      </c>
+      <c r="V5" s="8">
+        <f>$F5/$B5</f>
+        <v>1.8705832790123738</v>
+      </c>
+      <c r="W5" s="9">
+        <v>4077155</v>
+      </c>
+      <c r="X5" s="8">
+        <f>$H5/$B5</f>
+        <v>1.934279229657631</v>
+      </c>
+      <c r="Y5" s="9">
+        <v>4117917</v>
+      </c>
+      <c r="Z5" s="8">
+        <f>$J5/$B5</f>
+        <v>1.9536174912540882</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>3032688</v>
+      </c>
+      <c r="AB5" s="8">
+        <f>$L5/$B5</f>
+        <v>1.4387643855659011</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -41648,8 +41799,52 @@
         <f t="shared" ref="M6:M14" si="4">$L6/$B6</f>
         <v>1.5128824208463674</v>
       </c>
+      <c r="P6" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>2101546</v>
+      </c>
+      <c r="R6" s="3">
+        <v>-41373.800000000003</v>
+      </c>
+      <c r="S6" s="9">
+        <v>2059649</v>
+      </c>
+      <c r="T6" s="8">
+        <f t="shared" ref="T6:T14" si="5">$D6/$B6</f>
+        <v>0.98006372451519019</v>
+      </c>
+      <c r="U6" s="9">
+        <v>205399</v>
+      </c>
+      <c r="V6" s="8">
+        <f t="shared" ref="V6:V14" si="6">$F6/$B6</f>
+        <v>9.7737094500905522E-2</v>
+      </c>
+      <c r="W6" s="9">
+        <v>178275</v>
+      </c>
+      <c r="X6" s="8">
+        <f t="shared" ref="X6:X14" si="7">$H6/$B6</f>
+        <v>8.483040580601138E-2</v>
+      </c>
+      <c r="Y6" s="9">
+        <v>168372</v>
+      </c>
+      <c r="Z6" s="8">
+        <f t="shared" ref="Z6:Z14" si="8">$J6/$B6</f>
+        <v>8.0118160630316917E-2</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>3179392</v>
+      </c>
+      <c r="AB6" s="8">
+        <f t="shared" ref="AB6:AB14" si="9">$L6/$B6</f>
+        <v>1.5128824208463674</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -41694,8 +41889,52 @@
         <f t="shared" si="4"/>
         <v>1.5314663211560131</v>
       </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>2072295</v>
+      </c>
+      <c r="R7" s="3">
+        <v>-41039.9</v>
+      </c>
+      <c r="S7" s="9">
+        <v>2142109</v>
+      </c>
+      <c r="T7" s="8">
+        <f t="shared" si="5"/>
+        <v>1.0336892189577256</v>
+      </c>
+      <c r="U7" s="9">
+        <v>4002802</v>
+      </c>
+      <c r="V7" s="8">
+        <f t="shared" si="6"/>
+        <v>1.9315792394422608</v>
+      </c>
+      <c r="W7" s="9">
+        <v>4146900</v>
+      </c>
+      <c r="X7" s="8">
+        <f t="shared" si="7"/>
+        <v>2.0011147061591132</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>4192576</v>
+      </c>
+      <c r="Z7" s="8">
+        <f t="shared" si="8"/>
+        <v>2.023155969589272</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>3173650</v>
+      </c>
+      <c r="AB7" s="8">
+        <f t="shared" si="9"/>
+        <v>1.5314663211560131</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -41740,8 +41979,52 @@
         <f t="shared" si="4"/>
         <v>1.374375924837093</v>
       </c>
+      <c r="P8" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>2139566</v>
+      </c>
+      <c r="R8" s="3">
+        <v>-42039.1</v>
+      </c>
+      <c r="S8" s="9">
+        <v>2061589</v>
+      </c>
+      <c r="T8" s="8">
+        <f t="shared" si="5"/>
+        <v>0.96355475830144988</v>
+      </c>
+      <c r="U8" s="9">
+        <v>3385111</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="6"/>
+        <v>1.5821484357107938</v>
+      </c>
+      <c r="W8" s="9">
+        <v>3492527</v>
+      </c>
+      <c r="X8" s="8">
+        <f t="shared" si="7"/>
+        <v>1.6323530099094863</v>
+      </c>
+      <c r="Y8" s="9">
+        <v>3536357</v>
+      </c>
+      <c r="Z8" s="8">
+        <f t="shared" si="8"/>
+        <v>1.6528384728491665</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>2940568</v>
+      </c>
+      <c r="AB8" s="8">
+        <f t="shared" si="9"/>
+        <v>1.374375924837093</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -41786,8 +42069,52 @@
         <f t="shared" si="4"/>
         <v>1.4361889055196566</v>
       </c>
+      <c r="P9" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>2066451</v>
+      </c>
+      <c r="R9" s="3">
+        <v>-40570.6</v>
+      </c>
+      <c r="S9" s="9">
+        <v>2059366</v>
+      </c>
+      <c r="T9" s="8">
+        <f t="shared" si="5"/>
+        <v>0.99657141640426028</v>
+      </c>
+      <c r="U9" s="9">
+        <v>3620084</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="6"/>
+        <v>1.7518363609879934</v>
+      </c>
+      <c r="W9" s="9">
+        <v>3720841</v>
+      </c>
+      <c r="X9" s="8">
+        <f t="shared" si="7"/>
+        <v>1.8005948362675912</v>
+      </c>
+      <c r="Y9" s="9">
+        <v>3741750</v>
+      </c>
+      <c r="Z9" s="8">
+        <f t="shared" si="8"/>
+        <v>1.8107131502271285</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>2967814</v>
+      </c>
+      <c r="AB9" s="8">
+        <f t="shared" si="9"/>
+        <v>1.4361889055196566</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -41819,11 +42146,11 @@
         <v>0.50864262171506058</v>
       </c>
       <c r="J10" s="3">
-        <v>1022770</v>
+        <v>1022771</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="3"/>
-        <v>0.49676375247344895</v>
+        <v>0.49676423817771531</v>
       </c>
       <c r="L10" s="3">
         <v>544424</v>
@@ -41832,8 +42159,52 @@
         <f t="shared" si="4"/>
         <v>0.26442905949197276</v>
       </c>
+      <c r="P10" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2058866</v>
+      </c>
+      <c r="R10" s="3">
+        <v>-40118</v>
+      </c>
+      <c r="S10" s="9">
+        <v>1099011</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" si="5"/>
+        <v>0.53379433144264854</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1100834</v>
+      </c>
+      <c r="V10" s="8">
+        <f t="shared" si="6"/>
+        <v>0.53467977032016656</v>
+      </c>
+      <c r="W10" s="9">
+        <v>1047227</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" si="7"/>
+        <v>0.50864262171506058</v>
+      </c>
+      <c r="Y10" s="9">
+        <v>1022771</v>
+      </c>
+      <c r="Z10" s="8">
+        <f t="shared" si="8"/>
+        <v>0.49676423817771531</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>544424</v>
+      </c>
+      <c r="AB10" s="8">
+        <f t="shared" si="9"/>
+        <v>0.26442905949197276</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -41858,11 +42229,11 @@
         <v>6.2686174979938641E-2</v>
       </c>
       <c r="H11" s="3">
-        <v>127446</v>
+        <v>127447</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" si="2"/>
-        <v>6.224563106938371E-2</v>
+        <v>6.2246119477266812E-2</v>
       </c>
       <c r="J11" s="3">
         <v>128061</v>
@@ -41878,8 +42249,52 @@
         <f t="shared" si="4"/>
         <v>4.8312330980346957E-2</v>
       </c>
+      <c r="P11" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>2047469</v>
+      </c>
+      <c r="R11" s="3">
+        <v>-551445</v>
+      </c>
+      <c r="S11" s="9">
+        <v>392175</v>
+      </c>
+      <c r="T11" s="8">
+        <f t="shared" si="5"/>
+        <v>0.19154136155419202</v>
+      </c>
+      <c r="U11" s="9">
+        <v>128348</v>
+      </c>
+      <c r="V11" s="8">
+        <f t="shared" si="6"/>
+        <v>6.2686174979938641E-2</v>
+      </c>
+      <c r="W11" s="9">
+        <v>127447</v>
+      </c>
+      <c r="X11" s="8">
+        <f t="shared" si="7"/>
+        <v>6.2246119477266812E-2</v>
+      </c>
+      <c r="Y11" s="9">
+        <v>128061</v>
+      </c>
+      <c r="Z11" s="8">
+        <f t="shared" si="8"/>
+        <v>6.2546001917489352E-2</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>98918</v>
+      </c>
+      <c r="AB11" s="8">
+        <f t="shared" si="9"/>
+        <v>4.8312330980346957E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -41924,8 +42339,52 @@
         <f t="shared" si="4"/>
         <v>1.0784574404399869</v>
       </c>
+      <c r="P12" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2088062</v>
+      </c>
+      <c r="R12" s="3">
+        <v>-153915</v>
+      </c>
+      <c r="S12" s="9">
+        <v>2016836</v>
+      </c>
+      <c r="T12" s="8">
+        <f t="shared" si="5"/>
+        <v>0.96588894391066937</v>
+      </c>
+      <c r="U12" s="9">
+        <v>2983096</v>
+      </c>
+      <c r="V12" s="8">
+        <f t="shared" si="6"/>
+        <v>1.4286434023510797</v>
+      </c>
+      <c r="W12" s="9">
+        <v>3019744</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="7"/>
+        <v>1.4461946053326002</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>2985728</v>
+      </c>
+      <c r="Z12" s="8">
+        <f t="shared" si="8"/>
+        <v>1.4299039013209378</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>2251886</v>
+      </c>
+      <c r="AB12" s="8">
+        <f t="shared" si="9"/>
+        <v>1.0784574404399869</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -41970,8 +42429,52 @@
         <f t="shared" si="4"/>
         <v>1.4987874823767398</v>
       </c>
+      <c r="P13" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2143474</v>
+      </c>
+      <c r="R13" s="3">
+        <v>-46371.4</v>
+      </c>
+      <c r="S13" s="9">
+        <v>1993766</v>
+      </c>
+      <c r="T13" s="8">
+        <f t="shared" si="5"/>
+        <v>0.93015637231895509</v>
+      </c>
+      <c r="U13" s="9">
+        <v>2196928</v>
+      </c>
+      <c r="V13" s="8">
+        <f t="shared" si="6"/>
+        <v>1.024938021174971</v>
+      </c>
+      <c r="W13" s="9">
+        <v>2178405</v>
+      </c>
+      <c r="X13" s="8">
+        <f t="shared" si="7"/>
+        <v>1.0162964421308587</v>
+      </c>
+      <c r="Y13" s="9">
+        <v>2174183</v>
+      </c>
+      <c r="Z13" s="8">
+        <f t="shared" si="8"/>
+        <v>1.0143267424750662</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>3212612</v>
+      </c>
+      <c r="AB13" s="8">
+        <f t="shared" si="9"/>
+        <v>1.4987874823767398</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -42016,9 +42519,53 @@
         <f t="shared" si="4"/>
         <v>1.3905023055066421</v>
       </c>
+      <c r="P14" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>2054646</v>
+      </c>
+      <c r="R14" s="3">
+        <v>-42529.8</v>
+      </c>
+      <c r="S14" s="9">
+        <v>2100985</v>
+      </c>
+      <c r="T14" s="8">
+        <f t="shared" si="5"/>
+        <v>1.022553276817515</v>
+      </c>
+      <c r="U14" s="9">
+        <v>3870362</v>
+      </c>
+      <c r="V14" s="8">
+        <f t="shared" si="6"/>
+        <v>1.8837123280604056</v>
+      </c>
+      <c r="W14" s="9">
+        <v>3961523</v>
+      </c>
+      <c r="X14" s="8">
+        <f t="shared" si="7"/>
+        <v>1.9280805549958484</v>
+      </c>
+      <c r="Y14" s="9">
+        <v>3957700</v>
+      </c>
+      <c r="Z14" s="8">
+        <f t="shared" si="8"/>
+        <v>1.9262198938405934</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>2856990</v>
+      </c>
+      <c r="AB14" s="8">
+        <f t="shared" si="9"/>
+        <v>1.3905023055066421</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="16">
     <mergeCell ref="J1:K3"/>
     <mergeCell ref="L1:M3"/>
     <mergeCell ref="B1:B4"/>
@@ -42027,87 +42574,189 @@
     <mergeCell ref="D1:E3"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:I3"/>
+    <mergeCell ref="W1:X3"/>
+    <mergeCell ref="Y1:Z3"/>
+    <mergeCell ref="AA1:AB3"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="S1:T3"/>
+    <mergeCell ref="U1:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD49CBDD-CE66-4EE9-9CF9-B336109FE7BC}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q25" zoomScale="99" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="T1" zoomScale="131" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8"/>
+      <c r="M1" s="11"/>
+      <c r="P1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="10" t="str">
+        <f>D1</f>
+        <v>Алгоритм Хаффмана</v>
+      </c>
+      <c r="T1" s="10" t="str">
+        <f>F1</f>
+        <v>Алгоритм LZ77, окно 5 Кб</v>
+      </c>
+      <c r="U1" s="10" t="str">
+        <f>H1</f>
+        <v>Алгоритм LZ77, окно 10 Кб</v>
+      </c>
+      <c r="V1" s="10" t="str">
+        <f>J1</f>
+        <v>Алгоритм LZ77, окно 20 Кб</v>
+      </c>
+      <c r="W1" s="10" t="str">
+        <f>L1</f>
+        <v>Алгоритм LZW</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="10" t="str">
+        <f>S1</f>
+        <v>Алгоритм Хаффмана</v>
+      </c>
+      <c r="AD1" s="10" t="str">
+        <f t="shared" ref="AD1:AG1" si="0">T1</f>
+        <v>Алгоритм LZ77, окно 5 Кб</v>
+      </c>
+      <c r="AE1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Алгоритм LZ77, окно 10 Кб</v>
+      </c>
+      <c r="AF1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Алгоритм LZ77, окно 20 Кб</v>
+      </c>
+      <c r="AG1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Алгоритм LZW</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
@@ -42138,8 +42787,44 @@
       <c r="M4" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -42180,8 +42865,68 @@
       <c r="M5" s="5">
         <v>242204000</v>
       </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>2107842</v>
+      </c>
+      <c r="R5" s="3">
+        <f>'Коэффициенты сжатия файлов'!R5</f>
+        <v>-41251.9</v>
+      </c>
+      <c r="S5" s="5">
+        <f>D5</f>
+        <v>320061000</v>
+      </c>
+      <c r="T5" s="5">
+        <f>F5</f>
+        <v>2011920000</v>
+      </c>
+      <c r="U5" s="5">
+        <f>H5</f>
+        <v>4014850000</v>
+      </c>
+      <c r="V5" s="5">
+        <f>J5</f>
+        <v>6741920000</v>
+      </c>
+      <c r="W5" s="5">
+        <f>L5</f>
+        <v>695581000</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>2107842</v>
+      </c>
+      <c r="AB5" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB5</f>
+        <v>1.4387643855659011</v>
+      </c>
+      <c r="AC5" s="5">
+        <f>E5</f>
+        <v>1282810000</v>
+      </c>
+      <c r="AD5" s="5">
+        <f>G5</f>
+        <v>131025000</v>
+      </c>
+      <c r="AE5" s="5">
+        <f>I5</f>
+        <v>140000000</v>
+      </c>
+      <c r="AF5" s="5">
+        <f>K5</f>
+        <v>136002000</v>
+      </c>
+      <c r="AG5" s="5">
+        <f>M5</f>
+        <v>242204000</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -42222,8 +42967,68 @@
       <c r="M6" s="5">
         <v>229010000</v>
       </c>
+      <c r="P6" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>2101546</v>
+      </c>
+      <c r="R6" s="3">
+        <f>'Коэффициенты сжатия файлов'!R6</f>
+        <v>-41373.800000000003</v>
+      </c>
+      <c r="S6" s="5">
+        <f t="shared" ref="S6:S14" si="1">D6</f>
+        <v>288222000</v>
+      </c>
+      <c r="T6" s="5">
+        <f t="shared" ref="T6:T14" si="2">F6</f>
+        <v>123020000</v>
+      </c>
+      <c r="U6" s="5">
+        <f t="shared" ref="U6:U14" si="3">H6</f>
+        <v>193986000</v>
+      </c>
+      <c r="V6" s="5">
+        <f t="shared" ref="V6:V14" si="4">J6</f>
+        <v>290005000</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" ref="W6:W14" si="5">L6</f>
+        <v>638643000</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>2101546</v>
+      </c>
+      <c r="AB6" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB6</f>
+        <v>1.5128824208463674</v>
+      </c>
+      <c r="AC6" s="5">
+        <f t="shared" ref="AC6:AC14" si="6">E6</f>
+        <v>1416140000</v>
+      </c>
+      <c r="AD6" s="5">
+        <f t="shared" ref="AD6:AD14" si="7">G6</f>
+        <v>35847600</v>
+      </c>
+      <c r="AE6" s="5">
+        <f t="shared" ref="AE6:AE14" si="8">I6</f>
+        <v>37967000</v>
+      </c>
+      <c r="AF6" s="5">
+        <f t="shared" ref="AF6:AF14" si="9">K6</f>
+        <v>35987500</v>
+      </c>
+      <c r="AG6" s="5">
+        <f t="shared" ref="AG6:AG14" si="10">M6</f>
+        <v>229010000</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -42264,8 +43069,68 @@
       <c r="M7" s="5">
         <v>249013000</v>
       </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>2072295</v>
+      </c>
+      <c r="R7" s="3">
+        <f>'Коэффициенты сжатия файлов'!R7</f>
+        <v>-41039.9</v>
+      </c>
+      <c r="S7" s="5">
+        <f t="shared" si="1"/>
+        <v>296981000</v>
+      </c>
+      <c r="T7" s="5">
+        <f t="shared" si="2"/>
+        <v>2040460000</v>
+      </c>
+      <c r="U7" s="5">
+        <f t="shared" si="3"/>
+        <v>4028420000</v>
+      </c>
+      <c r="V7" s="5">
+        <f t="shared" si="4"/>
+        <v>6863410000</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" si="5"/>
+        <v>672706000</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>2072295</v>
+      </c>
+      <c r="AB7" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB7</f>
+        <v>1.5314663211560131</v>
+      </c>
+      <c r="AC7" s="5">
+        <f t="shared" si="6"/>
+        <v>1283560000</v>
+      </c>
+      <c r="AD7" s="5">
+        <f t="shared" si="7"/>
+        <v>131006000</v>
+      </c>
+      <c r="AE7" s="5">
+        <f t="shared" si="8"/>
+        <v>144999000</v>
+      </c>
+      <c r="AF7" s="5">
+        <f t="shared" si="9"/>
+        <v>137997000</v>
+      </c>
+      <c r="AG7" s="5">
+        <f t="shared" si="10"/>
+        <v>249013000</v>
+      </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -42306,8 +43171,68 @@
       <c r="M8" s="5">
         <v>237992000</v>
       </c>
+      <c r="P8" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>2139566</v>
+      </c>
+      <c r="R8" s="3">
+        <f>'Коэффициенты сжатия файлов'!R8</f>
+        <v>-42039.1</v>
+      </c>
+      <c r="S8" s="5">
+        <f t="shared" si="1"/>
+        <v>287008000</v>
+      </c>
+      <c r="T8" s="5">
+        <f t="shared" si="2"/>
+        <v>1732570000</v>
+      </c>
+      <c r="U8" s="5">
+        <f t="shared" si="3"/>
+        <v>3551360000</v>
+      </c>
+      <c r="V8" s="5">
+        <f t="shared" si="4"/>
+        <v>5793960000</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="5"/>
+        <v>676035000</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>4</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>2139566</v>
+      </c>
+      <c r="AB8" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB8</f>
+        <v>1.374375924837093</v>
+      </c>
+      <c r="AC8" s="5">
+        <f t="shared" si="6"/>
+        <v>1283720000</v>
+      </c>
+      <c r="AD8" s="5">
+        <f t="shared" si="7"/>
+        <v>117999000</v>
+      </c>
+      <c r="AE8" s="5">
+        <f t="shared" si="8"/>
+        <v>119000000</v>
+      </c>
+      <c r="AF8" s="5">
+        <f t="shared" si="9"/>
+        <v>124998000</v>
+      </c>
+      <c r="AG8" s="5">
+        <f t="shared" si="10"/>
+        <v>237992000</v>
+      </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -42348,12 +43273,69 @@
       <c r="M9" s="5">
         <v>229999000</v>
       </c>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="P9" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>2066451</v>
+      </c>
+      <c r="R9" s="3">
+        <f>'Коэффициенты сжатия файлов'!R9</f>
+        <v>-40570.6</v>
+      </c>
+      <c r="S9" s="5">
+        <f t="shared" si="1"/>
+        <v>286993000</v>
+      </c>
+      <c r="T9" s="5">
+        <f t="shared" si="2"/>
+        <v>1828880000</v>
+      </c>
+      <c r="U9" s="5">
+        <f t="shared" si="3"/>
+        <v>3676520000</v>
+      </c>
+      <c r="V9" s="5">
+        <f t="shared" si="4"/>
+        <v>6619920000</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="5"/>
+        <v>633008000</v>
+      </c>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="Z9" s="3">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>2066451</v>
+      </c>
+      <c r="AB9" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB9</f>
+        <v>1.4361889055196566</v>
+      </c>
+      <c r="AC9" s="5">
+        <f t="shared" si="6"/>
+        <v>1285070000</v>
+      </c>
+      <c r="AD9" s="5">
+        <f t="shared" si="7"/>
+        <v>119986000</v>
+      </c>
+      <c r="AE9" s="5">
+        <f t="shared" si="8"/>
+        <v>130001000</v>
+      </c>
+      <c r="AF9" s="5">
+        <f t="shared" si="9"/>
+        <v>179000000</v>
+      </c>
+      <c r="AG9" s="5">
+        <f t="shared" si="10"/>
+        <v>229999000</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -42394,12 +43376,69 @@
       <c r="M10" s="5">
         <v>80995700</v>
       </c>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+      <c r="P10" s="3">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2058866</v>
+      </c>
+      <c r="R10" s="3">
+        <f>'Коэффициенты сжатия файлов'!R10</f>
+        <v>-40118</v>
+      </c>
+      <c r="S10" s="5">
+        <f t="shared" si="1"/>
+        <v>161001000</v>
+      </c>
+      <c r="T10" s="5">
+        <f t="shared" si="2"/>
+        <v>1382150000</v>
+      </c>
+      <c r="U10" s="5">
+        <f t="shared" si="3"/>
+        <v>2460250000</v>
+      </c>
+      <c r="V10" s="5">
+        <f t="shared" si="4"/>
+        <v>4385090000</v>
+      </c>
+      <c r="W10" s="5">
+        <f t="shared" si="5"/>
+        <v>234002000</v>
+      </c>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+      <c r="Z10" s="3">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>2058866</v>
+      </c>
+      <c r="AB10" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB10</f>
+        <v>0.26442905949197276</v>
+      </c>
+      <c r="AC10" s="5">
+        <f t="shared" si="6"/>
+        <v>446042000</v>
+      </c>
+      <c r="AD10" s="5">
+        <f t="shared" si="7"/>
+        <v>58999400</v>
+      </c>
+      <c r="AE10" s="5">
+        <f t="shared" si="8"/>
+        <v>56000200</v>
+      </c>
+      <c r="AF10" s="5">
+        <f t="shared" si="9"/>
+        <v>57055900</v>
+      </c>
+      <c r="AG10" s="5">
+        <f t="shared" si="10"/>
+        <v>80995700</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -42440,12 +43479,69 @@
       <c r="M11" s="5">
         <v>48016300</v>
       </c>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
+      <c r="P11" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>2047469</v>
+      </c>
+      <c r="R11" s="3">
+        <f>'Коэффициенты сжатия файлов'!R11</f>
+        <v>-551445</v>
+      </c>
+      <c r="S11" s="5">
+        <f t="shared" si="1"/>
+        <v>69001600</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="2"/>
+        <v>1024420000</v>
+      </c>
+      <c r="U11" s="5">
+        <f t="shared" si="3"/>
+        <v>1702010000</v>
+      </c>
+      <c r="V11" s="5">
+        <f t="shared" si="4"/>
+        <v>2929710000</v>
+      </c>
+      <c r="W11" s="5">
+        <f t="shared" si="5"/>
+        <v>174002000</v>
+      </c>
       <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
+      <c r="Z11" s="3">
+        <v>7</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>2047469</v>
+      </c>
+      <c r="AB11" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB11</f>
+        <v>4.8312330980346957E-2</v>
+      </c>
+      <c r="AC11" s="5">
+        <f t="shared" si="6"/>
+        <v>311999000</v>
+      </c>
+      <c r="AD11" s="5">
+        <f t="shared" si="7"/>
+        <v>34000700</v>
+      </c>
+      <c r="AE11" s="5">
+        <f t="shared" si="8"/>
+        <v>33956200</v>
+      </c>
+      <c r="AF11" s="5">
+        <f t="shared" si="9"/>
+        <v>33954700</v>
+      </c>
+      <c r="AG11" s="5">
+        <f t="shared" si="10"/>
+        <v>48016300</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -42486,12 +43582,69 @@
       <c r="M12" s="5">
         <v>201337000</v>
       </c>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
+      <c r="P12" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2088062</v>
+      </c>
+      <c r="R12" s="3">
+        <f>'Коэффициенты сжатия файлов'!R12</f>
+        <v>-153915</v>
+      </c>
+      <c r="S12" s="5">
+        <f t="shared" si="1"/>
+        <v>273000000</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="2"/>
+        <v>1617110000</v>
+      </c>
+      <c r="U12" s="5">
+        <f t="shared" si="3"/>
+        <v>3117430000</v>
+      </c>
+      <c r="V12" s="5">
+        <f t="shared" si="4"/>
+        <v>5230600000</v>
+      </c>
+      <c r="W12" s="5">
+        <f t="shared" si="5"/>
+        <v>519978000</v>
+      </c>
       <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Z12" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>2088062</v>
+      </c>
+      <c r="AB12" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB12</f>
+        <v>1.0784574404399869</v>
+      </c>
+      <c r="AC12" s="5">
+        <f t="shared" si="6"/>
+        <v>1356120000</v>
+      </c>
+      <c r="AD12" s="5">
+        <f t="shared" si="7"/>
+        <v>115002000</v>
+      </c>
+      <c r="AE12" s="5">
+        <f t="shared" si="8"/>
+        <v>110147000</v>
+      </c>
+      <c r="AF12" s="5">
+        <f t="shared" si="9"/>
+        <v>109001000</v>
+      </c>
+      <c r="AG12" s="5">
+        <f t="shared" si="10"/>
+        <v>201337000</v>
+      </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -42532,12 +43685,69 @@
       <c r="M13" s="5">
         <v>208956000</v>
       </c>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
+      <c r="P13" s="3">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2143474</v>
+      </c>
+      <c r="R13" s="3">
+        <f>'Коэффициенты сжатия файлов'!R13</f>
+        <v>-46371.4</v>
+      </c>
+      <c r="S13" s="5">
+        <f t="shared" si="1"/>
+        <v>236988000</v>
+      </c>
+      <c r="T13" s="5">
+        <f t="shared" si="2"/>
+        <v>1530270000</v>
+      </c>
+      <c r="U13" s="5">
+        <f t="shared" si="3"/>
+        <v>2814140000</v>
+      </c>
+      <c r="V13" s="5">
+        <f t="shared" si="4"/>
+        <v>4896720000</v>
+      </c>
+      <c r="W13" s="5">
+        <f t="shared" si="5"/>
+        <v>576201000</v>
+      </c>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Z13" s="3">
+        <v>9</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>2143474</v>
+      </c>
+      <c r="AB13" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB13</f>
+        <v>1.4987874823767398</v>
+      </c>
+      <c r="AC13" s="5">
+        <f t="shared" si="6"/>
+        <v>1179790000</v>
+      </c>
+      <c r="AD13" s="5">
+        <f t="shared" si="7"/>
+        <v>91001100</v>
+      </c>
+      <c r="AE13" s="5">
+        <f t="shared" si="8"/>
+        <v>87999400</v>
+      </c>
+      <c r="AF13" s="5">
+        <f t="shared" si="9"/>
+        <v>87535700</v>
+      </c>
+      <c r="AG13" s="5">
+        <f t="shared" si="10"/>
+        <v>208956000</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -42578,18 +43788,75 @@
       <c r="M14" s="5">
         <v>241999000</v>
       </c>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
+      <c r="P14" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>2054646</v>
+      </c>
+      <c r="R14" s="3">
+        <f>'Коэффициенты сжатия файлов'!R14</f>
+        <v>-42529.8</v>
+      </c>
+      <c r="S14" s="5">
+        <f t="shared" si="1"/>
+        <v>331000000</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="2"/>
+        <v>1969040000</v>
+      </c>
+      <c r="U14" s="5">
+        <f t="shared" si="3"/>
+        <v>3922100000</v>
+      </c>
+      <c r="V14" s="5">
+        <f t="shared" si="4"/>
+        <v>6544650000</v>
+      </c>
+      <c r="W14" s="5">
+        <f t="shared" si="5"/>
+        <v>607114000</v>
+      </c>
       <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
+      <c r="Z14" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>2054646</v>
+      </c>
+      <c r="AB14" s="3">
+        <f>'Коэффициенты сжатия файлов'!AB14</f>
+        <v>1.3905023055066421</v>
+      </c>
+      <c r="AC14" s="5">
+        <f t="shared" si="6"/>
+        <v>1490340000</v>
+      </c>
+      <c r="AD14" s="5">
+        <f t="shared" si="7"/>
+        <v>130002000</v>
+      </c>
+      <c r="AE14" s="5">
+        <f t="shared" si="8"/>
+        <v>133967000</v>
+      </c>
+      <c r="AF14" s="5">
+        <f t="shared" si="9"/>
+        <v>134599000</v>
+      </c>
+      <c r="AG14" s="5">
+        <f t="shared" si="10"/>
+        <v>241999000</v>
+      </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="Y16" s="1"/>
@@ -42715,7 +43982,7 @@
       <c r="X29" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="24">
     <mergeCell ref="J1:K3"/>
     <mergeCell ref="L1:M3"/>
     <mergeCell ref="A1:A4"/>
@@ -42724,6 +43991,22 @@
     <mergeCell ref="D1:E3"/>
     <mergeCell ref="F1:G3"/>
     <mergeCell ref="H1:I3"/>
+    <mergeCell ref="Z1:Z4"/>
+    <mergeCell ref="AA1:AA4"/>
+    <mergeCell ref="AB1:AB4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="V1:V3"/>
+    <mergeCell ref="W1:W3"/>
+    <mergeCell ref="AC1:AC3"/>
+    <mergeCell ref="AD1:AD3"/>
+    <mergeCell ref="AE1:AE3"/>
+    <mergeCell ref="AF1:AF3"/>
+    <mergeCell ref="AG1:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>